<commit_message>
Risolti buchi di logica, implementate funzioni aggiuntive
</commit_message>
<xml_diff>
--- a/RinominaPdf/rinomina.xlsx
+++ b/RinominaPdf/rinomina.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Haider Maqsood\Desktop\Software\RinominaPdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A7E298-C68D-4ADB-B674-AAB0112F159F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F2405B-E153-4B32-88F8-C3DC8E406626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E3CF18D8-7B63-4772-892E-5AA85ED10D84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3CF18D8-7B63-4772-892E-5AA85ED10D84}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -27,22 +27,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>nuovo1.pdf</t>
-  </si>
-  <si>
-    <t>nuovo2.pdf</t>
-  </si>
-  <si>
-    <t>nuovo</t>
-  </si>
-  <si>
     <t>old</t>
   </si>
   <si>
-    <t>old1.pdf</t>
-  </si>
-  <si>
-    <t>old2.pdf</t>
+    <t>new</t>
+  </si>
+  <si>
+    <t>old1</t>
+  </si>
+  <si>
+    <t>nuovo2</t>
+  </si>
+  <si>
+    <t>nuovo1</t>
+  </si>
+  <si>
+    <t>old2</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,18 +408,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -427,7 +427,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>